<commit_message>
fix bubble chart scaling, update templates
</commit_message>
<xml_diff>
--- a/inst/app/www/FIND-CI_input_template.xlsx
+++ b/inst/app/www/FIND-CI_input_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42dcc5b33b6ca4b2/Work/COINrApp/FINDCompIndicatoR/www/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\becke\OneDrive\Work\COINrApp\composer\inst\app\www\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="130" documentId="8_{C7617BF7-6F09-49D4-B3E4-FF4118A21D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9007D7E2-19E2-437A-A079-CCF8F9EACD40}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6610720-C4DB-49F9-A3E6-E3DB6A1FEBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12240" yWindow="2595" windowWidth="25380" windowHeight="18150" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -289,7 +289,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="25">
   <si>
     <t>uName</t>
   </si>
@@ -297,12 +297,6 @@
     <t>uCode</t>
   </si>
   <si>
-    <t>Population</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Level</t>
   </si>
   <si>
@@ -318,9 +312,6 @@
     <t>Weight</t>
   </si>
   <si>
-    <t>Denominator</t>
-  </si>
-  <si>
     <t>Parent</t>
   </si>
   <si>
@@ -333,141 +324,6 @@
     <t>Aggregate</t>
   </si>
   <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>WB_REGION_group</t>
-  </si>
-  <si>
-    <t>Continent_group</t>
-  </si>
-  <si>
-    <t>Who_region_group</t>
-  </si>
-  <si>
-    <t>hiv_prevalence_rate_female_15_24</t>
-  </si>
-  <si>
-    <t>asr_cx_ca_incidence_rate</t>
-  </si>
-  <si>
-    <t>asr_cx_ca_mortality_rate</t>
-  </si>
-  <si>
-    <t>find_presence</t>
-  </si>
-  <si>
-    <t>income_fit</t>
-  </si>
-  <si>
-    <t>advocacy</t>
-  </si>
-  <si>
-    <t>partner_contracts_value</t>
-  </si>
-  <si>
-    <t>hpv_vacc_coverage_by_15_female</t>
-  </si>
-  <si>
-    <t>ict_indiv_using_internet_females</t>
-  </si>
-  <si>
-    <t>NCD_CCS_cervicalcancermethod</t>
-  </si>
-  <si>
-    <t>NCD_CCS_CancerPlan</t>
-  </si>
-  <si>
-    <t>NCD_CCS_CancerReg</t>
-  </si>
-  <si>
-    <t>NCD_CCS_cervicalcancerscreening</t>
-  </si>
-  <si>
-    <t>NCD_CCS_cervicalcancerpgmcvg</t>
-  </si>
-  <si>
-    <t>NCD_CCS_cervicalcancerpgmtype</t>
-  </si>
-  <si>
-    <t>CxCa mortality rate</t>
-  </si>
-  <si>
-    <t>epidemiological_impact</t>
-  </si>
-  <si>
-    <t>CxCa incidence rate</t>
-  </si>
-  <si>
-    <t>HIV prevalence rate (women 15-24)</t>
-  </si>
-  <si>
-    <t>HPV vaccination coverage (women by 15)</t>
-  </si>
-  <si>
-    <t>readiness</t>
-  </si>
-  <si>
-    <t>Coverage of national CxCa screening program</t>
-  </si>
-  <si>
-    <t>Type of national CxCa screening program</t>
-  </si>
-  <si>
-    <t>Existence of national CxCa screening program</t>
-  </si>
-  <si>
-    <t>Existence of population-based cancer registry</t>
-  </si>
-  <si>
-    <t>Existence of operational policy/strategy/action plan for cancer</t>
-  </si>
-  <si>
-    <t>Most widely used screening method in national CxCa screening program</t>
-  </si>
-  <si>
-    <t>Individuals using the Internet gender (females)</t>
-  </si>
-  <si>
-    <t>FIND presence</t>
-  </si>
-  <si>
-    <t>strategic_fit</t>
-  </si>
-  <si>
-    <t>Advocacy groups and civil societies</t>
-  </si>
-  <si>
-    <t>Partner contracts in country</t>
-  </si>
-  <si>
-    <t>Income fit</t>
-  </si>
-  <si>
-    <t>Epidemiological impact</t>
-  </si>
-  <si>
-    <t>cxca_prioritization_index</t>
-  </si>
-  <si>
-    <t>Country readiness</t>
-  </si>
-  <si>
-    <t>Strategic fit for FIND</t>
-  </si>
-  <si>
-    <t>Cervical cancer prioritization index</t>
-  </si>
-  <si>
-    <t>World bank region</t>
-  </si>
-  <si>
-    <t>Continent</t>
-  </si>
-  <si>
-    <t>WHO region</t>
-  </si>
-  <si>
     <t>&lt;Indicator or group code&gt;</t>
   </si>
   <si>
@@ -487,6 +343,27 @@
   </si>
   <si>
     <t>&lt;Add as many rows as you need…&gt;</t>
+  </si>
+  <si>
+    <t>ind_1</t>
+  </si>
+  <si>
+    <t>ind_2</t>
+  </si>
+  <si>
+    <t>Indicator 1</t>
+  </si>
+  <si>
+    <t>Indicator 2</t>
+  </si>
+  <si>
+    <t>Dim_1</t>
+  </si>
+  <si>
+    <t>Dimension_1</t>
+  </si>
+  <si>
+    <t>Index</t>
   </si>
 </sst>
 </file>
@@ -1128,27 +1005,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0"/>
-            <a:t>&lt;</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="1">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Link</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> to documentation</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>&gt;</a:t>
+            <a:t>https://finddx.github.io/composer/data_input.html </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1214,7 +1071,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t> for a clear example of how the finished template should look like.</a:t>
+            <a:t> for a clear example of how the finished template should look like (link on first page of app)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1223,23 +1080,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>&lt;</a:t>
+            <a:t>Note that in the following sheets you should delete everything except the table headers and fill in with your own data.</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" i="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>add link to example data set</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
-            <a:t>&gt;</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-GB" sz="1100" b="0" baseline="0"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1249,9 +1091,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1289,7 +1131,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1395,7 +1237,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1537,7 +1379,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1548,7 +1390,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S17" sqref="S17"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1562,7 +1404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1583,157 +1425,157 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="183" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1746,10 +1588,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1763,25 +1605,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1789,10 +1631,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1801,10 +1643,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1815,53 +1657,53 @@
         <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
+      <c r="A4" t="s">
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1870,21 +1712,21 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1892,386 +1734,8 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
       <c r="G6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>3</v>
-      </c>
-      <c r="B20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>2</v>
-      </c>
-      <c r="G24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>